<commit_message>
Continued working on dissertation and added optimised results
</commit_message>
<xml_diff>
--- a/Documentation/filebenchAveragedResultsExcel.xlsx
+++ b/Documentation/filebenchAveragedResultsExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/43d7ff6e475f4317/Documents/Uni_Temp/Third_Year/Dissertation/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{F7510D9F-0D75-41A7-89B5-7E7C340231DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F478DAC4-AC70-4152-91DD-6C339F9DECF6}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="8_{F7510D9F-0D75-41A7-89B5-7E7C340231DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79A68C61-6E4D-4C5B-8132-426A8500B149}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-7150" windowWidth="38620" windowHeight="21220" xr2:uid="{3BB8074F-2156-4486-902C-F8FF38704295}"/>
+    <workbookView xWindow="-38510" yWindow="-7150" windowWidth="38620" windowHeight="21220" activeTab="3" xr2:uid="{3BB8074F-2156-4486-902C-F8FF38704295}"/>
   </bookViews>
   <sheets>
     <sheet name="filebenchAveragedResults" sheetId="2" r:id="rId1"/>
@@ -1282,6 +1282,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'Fileserver mbs'!$A$2:$A$199</c:f>
@@ -1504,8 +1562,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1522,6 +1581,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Configurations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1587,6 +1701,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Speed</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> in mb/s</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1774,6 +1948,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'Fileserver ops'!$A$2:$A$199</c:f>
@@ -1996,8 +2228,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -2014,6 +2247,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Configurations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2079,6 +2367,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> of operations per second</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2266,109 +2614,167 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'Videoserver mbs'!$A$2:$A$199</c:f>
               <c:strCache>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>stripe/2/fileserver mb/s</c:v>
+                  <c:v>stripe/2/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>stripe/3/fileserver mb/s</c:v>
+                  <c:v>stripe/3/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>stripe/4/fileserver mb/s</c:v>
+                  <c:v>stripe/4/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>stripe/5/fileserver mb/s</c:v>
+                  <c:v>stripe/5/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>stripe/6/fileserver mb/s</c:v>
+                  <c:v>stripe/6/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>mirror/2/fileserver mb/s</c:v>
+                  <c:v>mirror/2/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>mirror/3/fileserver mb/s</c:v>
+                  <c:v>mirror/3/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>mirror/4/fileserver mb/s</c:v>
+                  <c:v>mirror/4/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>mirror/5/fileserver mb/s</c:v>
+                  <c:v>mirror/5/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>mirror/6/fileserver mb/s</c:v>
+                  <c:v>mirror/6/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>stripedmirror/4disk2vdev/fileserver mb/s</c:v>
+                  <c:v>stripedmirror/4disk2vdev/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>stripedmirror/5disk2vdev/fileserver mb/s</c:v>
+                  <c:v>stripedmirror/5disk2vdev/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>stripedmirror/6disk2vdev/fileserver mb/s</c:v>
+                  <c:v>stripedmirror/6disk2vdev/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>stripedmirror/6disk2vdevUneven/fileserver mb/s</c:v>
+                  <c:v>stripedmirror/6disk2vdevUneven/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>stripedmirror/6disk3vdev/fileserver mb/s</c:v>
+                  <c:v>stripedmirror/6disk3vdev/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>raidz/2/fileserver mb/s</c:v>
+                  <c:v>raidz/2/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>raidz/3/fileserver mb/s</c:v>
+                  <c:v>raidz/3/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>raidz/4/fileserver mb/s</c:v>
+                  <c:v>raidz/4/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>raidz/5/fileserver mb/s</c:v>
+                  <c:v>raidz/5/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>raidz/6/fileserver mb/s</c:v>
+                  <c:v>raidz/6/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>raidz/4disk2vdev/fileserver mb/s</c:v>
+                  <c:v>raidz/4disk2vdev/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>raidz/5disk2vdev/fileserver mb/s</c:v>
+                  <c:v>raidz/5disk2vdev/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>raidz/6disk2vdev/fileserver mb/s</c:v>
+                  <c:v>raidz/6disk2vdev/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>raidz/6disk2vdevUneven/fileserver mb/s</c:v>
+                  <c:v>raidz/6disk2vdevUneven/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>raidz/6disk3vdev/fileserver mb/s</c:v>
+                  <c:v>raidz/6disk3vdev/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>raidz2/3/fileserver mb/s</c:v>
+                  <c:v>raidz2/3/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>raidz2/4/fileserver mb/s</c:v>
+                  <c:v>raidz2/4/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>raidz2/5/fileserver mb/s</c:v>
+                  <c:v>raidz2/5/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>raidz2/6/fileserver mb/s</c:v>
+                  <c:v>raidz2/6/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>raidz2/6disk2vdev/fileserver mb/s</c:v>
+                  <c:v>raidz2/6disk2vdev/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>raidz3/4/fileserver mb/s</c:v>
+                  <c:v>raidz3/4/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>raidz3/5/fileserver mb/s</c:v>
+                  <c:v>raidz3/5/videoserver mb/s</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>raidz3/6/fileserver mb/s</c:v>
+                  <c:v>raidz3/6/videoserver mb/s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2380,103 +2786,103 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>26.74</c:v>
+                  <c:v>121.72</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.56</c:v>
+                  <c:v>128.08000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43.22</c:v>
+                  <c:v>144.28</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46.94</c:v>
+                  <c:v>164.78</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>48.36</c:v>
+                  <c:v>175.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.42</c:v>
+                  <c:v>98.12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27.36</c:v>
+                  <c:v>118.22</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30.26</c:v>
+                  <c:v>126.02</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32.36</c:v>
+                  <c:v>124.96</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>33.68</c:v>
+                  <c:v>123.84</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>37.200000000000003</c:v>
+                  <c:v>133.12</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>38.54</c:v>
+                  <c:v>133.32</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41.98</c:v>
+                  <c:v>134.06</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>38.6</c:v>
+                  <c:v>134.02000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>45.2</c:v>
+                  <c:v>147.69999999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>23.58</c:v>
+                  <c:v>88.52</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>25.78</c:v>
+                  <c:v>125.12</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>29.88</c:v>
+                  <c:v>127.3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>34.92</c:v>
+                  <c:v>130.32</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>34.18</c:v>
+                  <c:v>130.54</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>37.78</c:v>
+                  <c:v>130.4</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>34.799999999999997</c:v>
+                  <c:v>132.58000000000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>42.64</c:v>
+                  <c:v>136.80000000000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>35.68</c:v>
+                  <c:v>136.12</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>45.34</c:v>
+                  <c:v>147.68</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>26.88</c:v>
+                  <c:v>108.16</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>27.98</c:v>
+                  <c:v>101.76</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>33.4</c:v>
+                  <c:v>132.66</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>35.82</c:v>
+                  <c:v>130.66</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>43.22</c:v>
+                  <c:v>147.04</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>15.22</c:v>
+                  <c:v>73.16</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>34.36</c:v>
+                  <c:v>127.94</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>28.44</c:v>
+                  <c:v>123.78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2488,8 +2894,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -2506,6 +2913,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Configurations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2571,6 +3033,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Speed in mb/s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2697,7 +3214,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> mb/s</a:t>
+              <a:t> ops/s</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2763,109 +3280,167 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'Videoserver ops'!$A$2:$A$199</c:f>
               <c:strCache>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>stripe/2/fileserver ops/s</c:v>
+                  <c:v>stripe/2/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>stripe/3/fileserver ops/s</c:v>
+                  <c:v>stripe/3/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>stripe/4/fileserver ops/s</c:v>
+                  <c:v>stripe/4/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>stripe/5/fileserver ops/s</c:v>
+                  <c:v>stripe/5/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>stripe/6/fileserver ops/s</c:v>
+                  <c:v>stripe/6/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>mirror/2/fileserver ops/s</c:v>
+                  <c:v>mirror/2/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>mirror/3/fileserver ops/s</c:v>
+                  <c:v>mirror/3/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>mirror/4/fileserver ops/s</c:v>
+                  <c:v>mirror/4/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>mirror/5/fileserver ops/s</c:v>
+                  <c:v>mirror/5/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>mirror/6/fileserver ops/s</c:v>
+                  <c:v>mirror/6/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>stripedmirror/4disk2vdev/fileserver ops/s</c:v>
+                  <c:v>stripedmirror/4disk2vdev/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>stripedmirror/5disk2vdev/fileserver ops/s</c:v>
+                  <c:v>stripedmirror/5disk2vdev/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>stripedmirror/6disk2vdev/fileserver ops/s</c:v>
+                  <c:v>stripedmirror/6disk2vdev/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>stripedmirror/6disk2vdevUneven/fileserver ops/s</c:v>
+                  <c:v>stripedmirror/6disk2vdevUneven/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>stripedmirror/6disk3vdev/fileserver ops/s</c:v>
+                  <c:v>stripedmirror/6disk3vdev/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>raidz/2/fileserver ops/s</c:v>
+                  <c:v>raidz/2/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>raidz/3/fileserver ops/s</c:v>
+                  <c:v>raidz/3/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>raidz/4/fileserver ops/s</c:v>
+                  <c:v>raidz/4/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>raidz/5/fileserver ops/s</c:v>
+                  <c:v>raidz/5/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>raidz/6/fileserver ops/s</c:v>
+                  <c:v>raidz/6/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>raidz/4disk2vdev/fileserver ops/s</c:v>
+                  <c:v>raidz/4disk2vdev/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>raidz/5disk2vdev/fileserver ops/s</c:v>
+                  <c:v>raidz/5disk2vdev/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>raidz/6disk2vdev/fileserver ops/s</c:v>
+                  <c:v>raidz/6disk2vdev/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>raidz/6disk2vdevUneven/fileserver ops/s</c:v>
+                  <c:v>raidz/6disk2vdevUneven/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>raidz/6disk3vdev/fileserver ops/s</c:v>
+                  <c:v>raidz/6disk3vdev/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>raidz2/3/fileserver ops/s</c:v>
+                  <c:v>raidz2/3/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>raidz2/4/fileserver ops/s</c:v>
+                  <c:v>raidz2/4/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>raidz2/5/fileserver ops/s</c:v>
+                  <c:v>raidz2/5/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>raidz2/6/fileserver ops/s</c:v>
+                  <c:v>raidz2/6/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>raidz2/6disk2vdev/fileserver ops/s</c:v>
+                  <c:v>raidz2/6disk2vdev/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>raidz3/4/fileserver ops/s</c:v>
+                  <c:v>raidz3/4/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>raidz3/5/fileserver ops/s</c:v>
+                  <c:v>raidz3/5/videoserver ops/s</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>raidz3/6/fileserver ops/s</c:v>
+                  <c:v>raidz3/6/videoserver ops/s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2877,103 +3452,103 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>1125.7650000000001</c:v>
+                  <c:v>334.08300000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1534.0350000000001</c:v>
+                  <c:v>381.375</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1812.6659999999999</c:v>
+                  <c:v>383.483</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1967.587</c:v>
+                  <c:v>383.54199999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2025.5229999999999</c:v>
+                  <c:v>383.61099999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>987.41200000000003</c:v>
+                  <c:v>275.255</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1153.028</c:v>
+                  <c:v>361.149</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1271.1310000000001</c:v>
+                  <c:v>381.39499999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1361.816</c:v>
+                  <c:v>382.53500000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1417.6510000000001</c:v>
+                  <c:v>383.52499999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1562.481</c:v>
+                  <c:v>382.49099999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1616.33</c:v>
+                  <c:v>383.19900000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1757.136</c:v>
+                  <c:v>383.54</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1619.838</c:v>
+                  <c:v>383.31700000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1893.306</c:v>
+                  <c:v>383.56799999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>993.61800000000005</c:v>
+                  <c:v>250.739</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1084.441</c:v>
+                  <c:v>364.18099999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1255.857</c:v>
+                  <c:v>367.37</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1467.557</c:v>
+                  <c:v>382.20499999999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1436.2529999999999</c:v>
+                  <c:v>383.06599999999997</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1586.2840000000001</c:v>
+                  <c:v>382.435</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1462.694</c:v>
+                  <c:v>383.041</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1789.1769999999999</c:v>
+                  <c:v>383.54700000000003</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1498.6079999999999</c:v>
+                  <c:v>383.57400000000001</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1900.413</c:v>
+                  <c:v>383.44900000000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1132.9760000000001</c:v>
+                  <c:v>327.476</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1175.973</c:v>
+                  <c:v>243.84</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1403.7439999999999</c:v>
+                  <c:v>347.54399999999998</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1504.1679999999999</c:v>
+                  <c:v>383.48099999999999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1812.3689999999999</c:v>
+                  <c:v>383.57400000000001</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>644.63499999999999</c:v>
+                  <c:v>192.261</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1443.1590000000001</c:v>
+                  <c:v>383.51799999999997</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1197.0409999999999</c:v>
+                  <c:v>305.89800000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2985,8 +3560,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -3003,6 +3579,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Configurations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3068,6 +3699,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> of operations per second</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3255,6 +3946,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'Mongo mbs'!$A$2:$A$199</c:f>
@@ -3477,8 +4226,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -3495,6 +4245,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Configurations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3560,6 +4365,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Speed</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> in mb/s</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3747,6 +4612,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'Mongo ops'!$A$2:$A$199</c:f>
@@ -3969,8 +4892,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -3987,6 +4911,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Conigurations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4052,6 +5031,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of operations per second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -7665,6 +8699,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7984,7 +9022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA9DE6B3-8E76-42C9-8E41-8281E733174A}">
   <dimension ref="A1:B199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+    <sheetView topLeftCell="A79" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -9597,7 +10635,7 @@
   <dimension ref="A1:B199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W68" sqref="W68"/>
+      <selection activeCell="F212" sqref="F212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11217,7 +12255,7 @@
   <dimension ref="A1:B199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Z111" sqref="Z111"/>
+      <selection activeCell="X177" sqref="X177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12836,8 +13874,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:B199"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y146" sqref="Y146"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12853,7 +13891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -12869,7 +13907,7 @@
         <v>1125.7650000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -12901,7 +13939,7 @@
         <v>185.72800000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -12917,7 +13955,7 @@
         <v>1534.0350000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -12949,7 +13987,7 @@
         <v>190.08099999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -12965,7 +14003,7 @@
         <v>1812.6659999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -12997,7 +14035,7 @@
         <v>200.512</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -13013,7 +14051,7 @@
         <v>1967.587</v>
       </c>
     </row>
-    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -13045,7 +14083,7 @@
         <v>211.55199999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -13061,7 +14099,7 @@
         <v>2025.5229999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -13093,7 +14131,7 @@
         <v>223.62</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -13109,7 +14147,7 @@
         <v>987.41200000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -13141,7 +14179,7 @@
         <v>174.52</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -13157,7 +14195,7 @@
         <v>1153.028</v>
       </c>
     </row>
-    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -13189,7 +14227,7 @@
         <v>182.56200000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -13205,7 +14243,7 @@
         <v>1271.1310000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -13237,7 +14275,7 @@
         <v>190.13800000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -13253,7 +14291,7 @@
         <v>1361.816</v>
       </c>
     </row>
-    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -13285,7 +14323,7 @@
         <v>197.273</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -13301,7 +14339,7 @@
         <v>1417.6510000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -13333,7 +14371,7 @@
         <v>203.536</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -13349,7 +14387,7 @@
         <v>1562.481</v>
       </c>
     </row>
-    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -13381,7 +14419,7 @@
         <v>190.434</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -13397,7 +14435,7 @@
         <v>1616.33</v>
       </c>
     </row>
-    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -13429,7 +14467,7 @@
         <v>196.7</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -13445,7 +14483,7 @@
         <v>1757.136</v>
       </c>
     </row>
-    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -13477,7 +14515,7 @@
         <v>203.649</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -13493,7 +14531,7 @@
         <v>1619.838</v>
       </c>
     </row>
-    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -13525,7 +14563,7 @@
         <v>199.70099999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>86</v>
       </c>
@@ -13541,7 +14579,7 @@
         <v>1893.306</v>
       </c>
     </row>
-    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>88</v>
       </c>
@@ -13573,7 +14611,7 @@
         <v>203.94300000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>92</v>
       </c>
@@ -13589,7 +14627,7 @@
         <v>993.61800000000005</v>
       </c>
     </row>
-    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>94</v>
       </c>
@@ -13621,7 +14659,7 @@
         <v>174.26599999999999</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>98</v>
       </c>
@@ -13637,7 +14675,7 @@
         <v>1084.441</v>
       </c>
     </row>
-    <row r="100" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>100</v>
       </c>
@@ -13669,7 +14707,7 @@
         <v>159.79</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>104</v>
       </c>
@@ -13685,7 +14723,7 @@
         <v>1255.857</v>
       </c>
     </row>
-    <row r="106" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>106</v>
       </c>
@@ -13717,7 +14755,7 @@
         <v>164.79499999999999</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>110</v>
       </c>
@@ -13733,7 +14771,7 @@
         <v>1467.557</v>
       </c>
     </row>
-    <row r="112" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>112</v>
       </c>
@@ -13765,7 +14803,7 @@
         <v>166.48699999999999</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>116</v>
       </c>
@@ -13781,7 +14819,7 @@
         <v>1436.2529999999999</v>
       </c>
     </row>
-    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>118</v>
       </c>
@@ -13813,7 +14851,7 @@
         <v>163.4</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>122</v>
       </c>
@@ -13829,7 +14867,7 @@
         <v>1586.2840000000001</v>
       </c>
     </row>
-    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>124</v>
       </c>
@@ -13861,7 +14899,7 @@
         <v>190.51</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>128</v>
       </c>
@@ -13877,7 +14915,7 @@
         <v>1462.694</v>
       </c>
     </row>
-    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>130</v>
       </c>
@@ -13909,7 +14947,7 @@
         <v>178.69499999999999</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>134</v>
       </c>
@@ -13925,7 +14963,7 @@
         <v>1789.1769999999999</v>
       </c>
     </row>
-    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>136</v>
       </c>
@@ -13957,7 +14995,7 @@
         <v>171.67400000000001</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>140</v>
       </c>
@@ -13973,7 +15011,7 @@
         <v>1498.6079999999999</v>
       </c>
     </row>
-    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>142</v>
       </c>
@@ -14005,7 +15043,7 @@
         <v>175.73400000000001</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>146</v>
       </c>
@@ -14021,7 +15059,7 @@
         <v>1900.413</v>
       </c>
     </row>
-    <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>148</v>
       </c>
@@ -14053,7 +15091,7 @@
         <v>198.785</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>152</v>
       </c>
@@ -14069,7 +15107,7 @@
         <v>1132.9760000000001</v>
       </c>
     </row>
-    <row r="154" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>154</v>
       </c>
@@ -14101,7 +15139,7 @@
         <v>196.90600000000001</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>158</v>
       </c>
@@ -14117,7 +15155,7 @@
         <v>1175.973</v>
       </c>
     </row>
-    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>160</v>
       </c>
@@ -14149,7 +15187,7 @@
         <v>157.84899999999999</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>164</v>
       </c>
@@ -14165,7 +15203,7 @@
         <v>1403.7439999999999</v>
       </c>
     </row>
-    <row r="166" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>166</v>
       </c>
@@ -14197,7 +15235,7 @@
         <v>155.24600000000001</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>170</v>
       </c>
@@ -14213,7 +15251,7 @@
         <v>1504.1679999999999</v>
       </c>
     </row>
-    <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>172</v>
       </c>
@@ -14245,7 +15283,7 @@
         <v>169.917</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>176</v>
       </c>
@@ -14261,7 +15299,7 @@
         <v>1812.3689999999999</v>
       </c>
     </row>
-    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>178</v>
       </c>
@@ -14293,7 +15331,7 @@
         <v>213.48500000000001</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>182</v>
       </c>
@@ -14309,7 +15347,7 @@
         <v>644.63499999999999</v>
       </c>
     </row>
-    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>184</v>
       </c>
@@ -14341,7 +15379,7 @@
         <v>169.191</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>188</v>
       </c>
@@ -14357,7 +15395,7 @@
         <v>1443.1590000000001</v>
       </c>
     </row>
-    <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>190</v>
       </c>
@@ -14389,7 +15427,7 @@
         <v>158.37700000000001</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>194</v>
       </c>
@@ -14405,7 +15443,7 @@
         <v>1197.0409999999999</v>
       </c>
     </row>
-    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>196</v>
       </c>
@@ -14441,7 +15479,7 @@
   <autoFilter ref="A1:B199" xr:uid="{1BB5598E-6B14-4592-A393-93495B3E2FAB}">
     <filterColumn colId="0">
       <customFilters and="1">
-        <customFilter val="*fileserver*"/>
+        <customFilter val="*videoserver*"/>
         <customFilter val="*mb/s*"/>
       </customFilters>
     </filterColumn>
@@ -14457,7 +15495,7 @@
   <dimension ref="A1:B199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Y201" sqref="Y201"/>
+      <selection activeCell="W129" sqref="W129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14481,7 +15519,7 @@
         <v>26.74</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -14497,7 +15535,7 @@
         <v>121.72</v>
       </c>
     </row>
-    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -14529,7 +15567,7 @@
         <v>36.56</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -14545,7 +15583,7 @@
         <v>128.08000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -14577,7 +15615,7 @@
         <v>43.22</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -14593,7 +15631,7 @@
         <v>144.28</v>
       </c>
     </row>
-    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -14625,7 +15663,7 @@
         <v>46.94</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -14641,7 +15679,7 @@
         <v>164.78</v>
       </c>
     </row>
-    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -14673,7 +15711,7 @@
         <v>48.36</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -14689,7 +15727,7 @@
         <v>175.7</v>
       </c>
     </row>
-    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -14721,7 +15759,7 @@
         <v>23.42</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -14737,7 +15775,7 @@
         <v>98.12</v>
       </c>
     </row>
-    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -14769,7 +15807,7 @@
         <v>27.36</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -14785,7 +15823,7 @@
         <v>118.22</v>
       </c>
     </row>
-    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -14817,7 +15855,7 @@
         <v>30.26</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -14833,7 +15871,7 @@
         <v>126.02</v>
       </c>
     </row>
-    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -14865,7 +15903,7 @@
         <v>32.36</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -14881,7 +15919,7 @@
         <v>124.96</v>
       </c>
     </row>
-    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -14913,7 +15951,7 @@
         <v>33.68</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -14929,7 +15967,7 @@
         <v>123.84</v>
       </c>
     </row>
-    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -14961,7 +15999,7 @@
         <v>37.200000000000003</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -14977,7 +16015,7 @@
         <v>133.12</v>
       </c>
     </row>
-    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -15009,7 +16047,7 @@
         <v>38.54</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -15025,7 +16063,7 @@
         <v>133.32</v>
       </c>
     </row>
-    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -15057,7 +16095,7 @@
         <v>41.98</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -15073,7 +16111,7 @@
         <v>134.06</v>
       </c>
     </row>
-    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -15105,7 +16143,7 @@
         <v>38.6</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -15121,7 +16159,7 @@
         <v>134.02000000000001</v>
       </c>
     </row>
-    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>83</v>
       </c>
@@ -15153,7 +16191,7 @@
         <v>45.2</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>87</v>
       </c>
@@ -15169,7 +16207,7 @@
         <v>147.69999999999999</v>
       </c>
     </row>
-    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>89</v>
       </c>
@@ -15201,7 +16239,7 @@
         <v>23.58</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>93</v>
       </c>
@@ -15217,7 +16255,7 @@
         <v>88.52</v>
       </c>
     </row>
-    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>95</v>
       </c>
@@ -15249,7 +16287,7 @@
         <v>25.78</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>99</v>
       </c>
@@ -15265,7 +16303,7 @@
         <v>125.12</v>
       </c>
     </row>
-    <row r="101" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>101</v>
       </c>
@@ -15297,7 +16335,7 @@
         <v>29.88</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>105</v>
       </c>
@@ -15313,7 +16351,7 @@
         <v>127.3</v>
       </c>
     </row>
-    <row r="107" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>107</v>
       </c>
@@ -15345,7 +16383,7 @@
         <v>34.92</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>111</v>
       </c>
@@ -15361,7 +16399,7 @@
         <v>130.32</v>
       </c>
     </row>
-    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>113</v>
       </c>
@@ -15393,7 +16431,7 @@
         <v>34.18</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>117</v>
       </c>
@@ -15409,7 +16447,7 @@
         <v>130.54</v>
       </c>
     </row>
-    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>119</v>
       </c>
@@ -15441,7 +16479,7 @@
         <v>37.78</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>123</v>
       </c>
@@ -15457,7 +16495,7 @@
         <v>130.4</v>
       </c>
     </row>
-    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>125</v>
       </c>
@@ -15489,7 +16527,7 @@
         <v>34.799999999999997</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>129</v>
       </c>
@@ -15505,7 +16543,7 @@
         <v>132.58000000000001</v>
       </c>
     </row>
-    <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>131</v>
       </c>
@@ -15537,7 +16575,7 @@
         <v>42.64</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>135</v>
       </c>
@@ -15553,7 +16591,7 @@
         <v>136.80000000000001</v>
       </c>
     </row>
-    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>137</v>
       </c>
@@ -15585,7 +16623,7 @@
         <v>35.68</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>141</v>
       </c>
@@ -15601,7 +16639,7 @@
         <v>136.12</v>
       </c>
     </row>
-    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>143</v>
       </c>
@@ -15633,7 +16671,7 @@
         <v>45.34</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>147</v>
       </c>
@@ -15649,7 +16687,7 @@
         <v>147.68</v>
       </c>
     </row>
-    <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>149</v>
       </c>
@@ -15681,7 +16719,7 @@
         <v>26.88</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>153</v>
       </c>
@@ -15697,7 +16735,7 @@
         <v>108.16</v>
       </c>
     </row>
-    <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>155</v>
       </c>
@@ -15729,7 +16767,7 @@
         <v>27.98</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>159</v>
       </c>
@@ -15745,7 +16783,7 @@
         <v>101.76</v>
       </c>
     </row>
-    <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>161</v>
       </c>
@@ -15777,7 +16815,7 @@
         <v>33.4</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>165</v>
       </c>
@@ -15793,7 +16831,7 @@
         <v>132.66</v>
       </c>
     </row>
-    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>167</v>
       </c>
@@ -15825,7 +16863,7 @@
         <v>35.82</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>171</v>
       </c>
@@ -15841,7 +16879,7 @@
         <v>130.66</v>
       </c>
     </row>
-    <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>173</v>
       </c>
@@ -15873,7 +16911,7 @@
         <v>43.22</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>177</v>
       </c>
@@ -15889,7 +16927,7 @@
         <v>147.04</v>
       </c>
     </row>
-    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>179</v>
       </c>
@@ -15921,7 +16959,7 @@
         <v>15.22</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>183</v>
       </c>
@@ -15937,7 +16975,7 @@
         <v>73.16</v>
       </c>
     </row>
-    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>185</v>
       </c>
@@ -15969,7 +17007,7 @@
         <v>34.36</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>189</v>
       </c>
@@ -15985,7 +17023,7 @@
         <v>127.94</v>
       </c>
     </row>
-    <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>191</v>
       </c>
@@ -16017,7 +17055,7 @@
         <v>28.44</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>195</v>
       </c>
@@ -16033,7 +17071,7 @@
         <v>123.78</v>
       </c>
     </row>
-    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>197</v>
       </c>
@@ -16061,7 +17099,7 @@
   <autoFilter ref="A1:B199" xr:uid="{1BB5598E-6B14-4592-A393-93495B3E2FAB}">
     <filterColumn colId="0">
       <customFilters and="1">
-        <customFilter val="*fileserver*"/>
+        <customFilter val="*videoserver*"/>
         <customFilter val="*ops/s*"/>
       </customFilters>
     </filterColumn>
@@ -17697,7 +18735,7 @@
   <dimension ref="A1:B199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X91" sqref="X91"/>
+      <selection activeCell="I213" sqref="I213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>